<commit_message>
added code for NanoClass2 run
</commit_message>
<xml_diff>
--- a/results/data_summary.xlsx
+++ b/results/data_summary.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/n_dombrowski_uva_nl/Documents/Teaching/2024/MicEco/data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/n_dombrowski_uva_nl/Documents/Teaching/2024/MicEco/data_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACBB8A90-8629-4318-9F56-F34ECBF2EDE1}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AFAA8DE-E3AE-4FC2-B638-C9FD3B05D3C4}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="75" windowWidth="22650" windowHeight="15180" activeTab="1" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
+    <workbookView xWindow="2130" yWindow="105" windowWidth="22650" windowHeight="15180" activeTab="1" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="mapping_file" sheetId="3" r:id="rId2"/>
     <sheet name="seqkit_raw" sheetId="2" r:id="rId3"/>
+    <sheet name="seqkit_filtered" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="129">
   <si>
     <t>Barcode</t>
   </si>
@@ -361,27 +362,18 @@
     <t>BC22</t>
   </si>
   <si>
-    <t>BC2</t>
-  </si>
-  <si>
     <t>BC17</t>
   </si>
   <si>
     <t>BC18</t>
   </si>
   <si>
-    <t>BC1</t>
-  </si>
-  <si>
     <t>BC16</t>
   </si>
   <si>
     <t>BC20</t>
   </si>
   <si>
-    <t>BC3</t>
-  </si>
-  <si>
     <t>BC15</t>
   </si>
   <si>
@@ -400,18 +392,6 @@
     <t>BC24</t>
   </si>
   <si>
-    <t>BC5</t>
-  </si>
-  <si>
-    <t>BC6</t>
-  </si>
-  <si>
-    <t>BC7</t>
-  </si>
-  <si>
-    <t>BC9</t>
-  </si>
-  <si>
     <t>BC11</t>
   </si>
   <si>
@@ -419,6 +399,33 @@
   </si>
   <si>
     <t>BC14</t>
+  </si>
+  <si>
+    <t>BC01</t>
+  </si>
+  <si>
+    <t>BC02</t>
+  </si>
+  <si>
+    <t>BC03</t>
+  </si>
+  <si>
+    <t>BC05</t>
+  </si>
+  <si>
+    <t>BC06</t>
+  </si>
+  <si>
+    <t>BC07</t>
+  </si>
+  <si>
+    <t>BC09</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -472,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -488,6 +495,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -827,7 +837,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1637,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E22"/>
+      <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1684,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -1691,7 +1701,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -1708,7 +1718,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -1725,7 +1735,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1742,7 +1752,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -1759,7 +1769,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
@@ -1776,7 +1786,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -1793,7 +1803,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -1810,7 +1820,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -1827,7 +1837,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
@@ -1844,7 +1854,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1861,7 +1871,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
@@ -1878,7 +1888,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
@@ -1895,7 +1905,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>25</v>
@@ -1912,7 +1922,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>27</v>
@@ -1929,7 +1939,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
@@ -1946,7 +1956,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -1963,7 +1973,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>32</v>
@@ -1980,7 +1990,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>33</v>
@@ -1997,7 +2007,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
@@ -2023,13 +2033,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760AAF3-A183-4133-AF68-A9D427019BD9}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3207,21 +3217,1435 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="6">
+        <f>AVERAGE(D2:D23)</f>
+        <v>19695.904761904763</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" ref="E24:Q24" si="0">AVERAGE(E2:E23)</f>
+        <v>26715804.285714287</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>72.428571428571431</v>
+      </c>
       <c r="G24" s="6">
-        <f>AVERAGE(G2:G23)</f>
+        <f t="shared" si="0"/>
         <v>1358.4714285714285</v>
       </c>
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>3933.2380952380954</v>
+      </c>
       <c r="I24" s="6">
-        <f>AVERAGE(I2:I23)</f>
+        <f t="shared" si="0"/>
         <v>1374.6428571428571</v>
       </c>
       <c r="J24" s="6">
-        <f>AVERAGE(J2:J23)</f>
+        <f t="shared" si="0"/>
         <v>1425.547619047619</v>
       </c>
       <c r="K24" s="6">
-        <f>AVERAGE(K2:K23)</f>
+        <f t="shared" si="0"/>
         <v>1454.3571428571429</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="0"/>
+        <v>1430.3333333333333</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" si="0"/>
+        <v>51.139523809523816</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="0"/>
+        <v>10.698571428571428</v>
+      </c>
+      <c r="P24" s="6">
+        <f t="shared" si="0"/>
+        <v>12.172380952380951</v>
+      </c>
+      <c r="Q24" s="6">
+        <f t="shared" si="0"/>
+        <v>53.006666666666661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="5">
+        <f>SUM(D2:D22)</f>
+        <v>413614</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" ref="E25:Q25" si="1">SUM(E2:E22)</f>
+        <v>561031890</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="1"/>
+        <v>1521</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="1"/>
+        <v>28527.9</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="1"/>
+        <v>82598</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="1"/>
+        <v>28867.5</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="1"/>
+        <v>29936.5</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="1"/>
+        <v>30541.5</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" si="1"/>
+        <v>30037</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="1"/>
+        <v>1073.93</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="1"/>
+        <v>224.67</v>
+      </c>
+      <c r="P25" s="5">
+        <f t="shared" si="1"/>
+        <v>255.61999999999998</v>
+      </c>
+      <c r="Q25" s="5">
+        <f t="shared" si="1"/>
+        <v>1113.1399999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64606F4B-74B8-49A9-B4AF-97DC0E2C0EB5}">
+  <dimension ref="A1:Q25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="17" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="7">
+        <v>56120</v>
+      </c>
+      <c r="E2" s="7">
+        <v>80000338</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1425.5</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1599</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1402</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1431</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1455</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1432</v>
+      </c>
+      <c r="N2" s="6">
+        <v>49.67</v>
+      </c>
+      <c r="O2" s="6">
+        <v>9.94</v>
+      </c>
+      <c r="P2" s="6">
+        <v>12.07</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>52.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="7">
+        <v>71245</v>
+      </c>
+      <c r="E3" s="7">
+        <v>100660819</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1412.9</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1599</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1394</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1420</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1439</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1421</v>
+      </c>
+      <c r="N3" s="6">
+        <v>50.01</v>
+      </c>
+      <c r="O3" s="6">
+        <v>10.94</v>
+      </c>
+      <c r="P3" s="6">
+        <v>12.11</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>51.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="7">
+        <v>22725</v>
+      </c>
+      <c r="E4" s="7">
+        <v>32249707</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1419.1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1408</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1436</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1459</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1437</v>
+      </c>
+      <c r="N4" s="6">
+        <v>48.71</v>
+      </c>
+      <c r="O4" s="6">
+        <v>9.4</v>
+      </c>
+      <c r="P4" s="6">
+        <v>11.98</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>53.07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4518</v>
+      </c>
+      <c r="E5" s="7">
+        <v>6421323</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1101</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1421.3</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1586</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1394</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1427</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1456</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1429</v>
+      </c>
+      <c r="N5" s="6">
+        <v>49.89</v>
+      </c>
+      <c r="O5" s="6">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="P5" s="6">
+        <v>12.11</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>52.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="7">
+        <v>16637</v>
+      </c>
+      <c r="E6" s="7">
+        <v>23572157</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1416.9</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1389</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1420</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1453</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1422</v>
+      </c>
+      <c r="N6" s="6">
+        <v>49.91</v>
+      </c>
+      <c r="O6" s="6">
+        <v>10.43</v>
+      </c>
+      <c r="P6" s="6">
+        <v>12.11</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>52.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="7">
+        <v>17385</v>
+      </c>
+      <c r="E7" s="7">
+        <v>24489002</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1408.6</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1592</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1384</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1407</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1443</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1409</v>
+      </c>
+      <c r="N7" s="6">
+        <v>50.15</v>
+      </c>
+      <c r="O7" s="6">
+        <v>10.51</v>
+      </c>
+      <c r="P7" s="6">
+        <v>12.12</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>52.41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="7">
+        <v>11294</v>
+      </c>
+      <c r="E8" s="7">
+        <v>15801637</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1399.1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1383</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1407</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1431</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1408</v>
+      </c>
+      <c r="N8" s="6">
+        <v>52.31</v>
+      </c>
+      <c r="O8" s="6">
+        <v>11.16</v>
+      </c>
+      <c r="P8" s="6">
+        <v>12.33</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>53.37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="7">
+        <v>14264</v>
+      </c>
+      <c r="E9" s="7">
+        <v>20239535</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1418.9</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1596</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1394</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1430</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1456</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1431</v>
+      </c>
+      <c r="N9" s="6">
+        <v>52.09</v>
+      </c>
+      <c r="O9" s="6">
+        <v>11.22</v>
+      </c>
+      <c r="P9" s="6">
+        <v>12.3</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>52.93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="7">
+        <v>11187</v>
+      </c>
+      <c r="E10" s="7">
+        <v>15434727</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1379.7</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1587</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1366</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1397</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1424</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1398</v>
+      </c>
+      <c r="N10" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="O10" s="6">
+        <v>10.66</v>
+      </c>
+      <c r="P10" s="6">
+        <v>12.21</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>53.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="7">
+        <v>6569</v>
+      </c>
+      <c r="E11" s="7">
+        <v>9213293</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1402.5</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1380</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1408</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1443</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1410</v>
+      </c>
+      <c r="N11" s="6">
+        <v>52.1</v>
+      </c>
+      <c r="O11" s="6">
+        <v>11.19</v>
+      </c>
+      <c r="P11" s="6">
+        <v>12.28</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>52.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9865</v>
+      </c>
+      <c r="E12" s="7">
+        <v>13930265</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1412.1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1594</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1393</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1428</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1453</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1429</v>
+      </c>
+      <c r="N12" s="6">
+        <v>51.43</v>
+      </c>
+      <c r="O12" s="6">
+        <v>10.64</v>
+      </c>
+      <c r="P12" s="6">
+        <v>12.24</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>54.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="7">
+        <v>6268</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8870479</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1101</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1415.2</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1589</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1388</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1422</v>
+      </c>
+      <c r="K13" s="6">
+        <v>1454</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1424</v>
+      </c>
+      <c r="N13" s="6">
+        <v>52.13</v>
+      </c>
+      <c r="O13" s="6">
+        <v>11.43</v>
+      </c>
+      <c r="P13" s="6">
+        <v>12.31</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>52.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="7">
+        <v>13528</v>
+      </c>
+      <c r="E14" s="7">
+        <v>19294186</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1426.2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1598</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1406</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1431</v>
+      </c>
+      <c r="K14" s="6">
+        <v>1458</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1433</v>
+      </c>
+      <c r="N14" s="6">
+        <v>51.85</v>
+      </c>
+      <c r="O14" s="6">
+        <v>10.63</v>
+      </c>
+      <c r="P14" s="6">
+        <v>12.27</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>53.21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="7">
+        <v>17115</v>
+      </c>
+      <c r="E15" s="7">
+        <v>24403578</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1425.9</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1409</v>
+      </c>
+      <c r="J15" s="6">
+        <v>1434</v>
+      </c>
+      <c r="K15" s="6">
+        <v>1453</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6">
+        <v>1435</v>
+      </c>
+      <c r="N15" s="6">
+        <v>51.83</v>
+      </c>
+      <c r="O15" s="6">
+        <v>10.88</v>
+      </c>
+      <c r="P15" s="6">
+        <v>12.27</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>53.55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="7">
+        <v>15391</v>
+      </c>
+      <c r="E16" s="7">
+        <v>21987342</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1428.6</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1404</v>
+      </c>
+      <c r="J16" s="6">
+        <v>1438</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1463</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>1439</v>
+      </c>
+      <c r="N16" s="6">
+        <v>51.85</v>
+      </c>
+      <c r="O16" s="6">
+        <v>10.57</v>
+      </c>
+      <c r="P16" s="6">
+        <v>12.28</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>53.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="7">
+        <v>26013</v>
+      </c>
+      <c r="E17" s="7">
+        <v>36796768</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1414.6</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1599</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1396</v>
+      </c>
+      <c r="J17" s="6">
+        <v>1422</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1448</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="6">
+        <v>1423</v>
+      </c>
+      <c r="N17" s="6">
+        <v>51.53</v>
+      </c>
+      <c r="O17" s="6">
+        <v>11.01</v>
+      </c>
+      <c r="P17" s="6">
+        <v>12.25</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>52.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="7">
+        <v>3</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4404</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1421</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1468</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1518</v>
+      </c>
+      <c r="I18" s="6">
+        <v>1443</v>
+      </c>
+      <c r="J18" s="6">
+        <v>1465</v>
+      </c>
+      <c r="K18" s="6">
+        <v>1491.5</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6">
+        <v>1465</v>
+      </c>
+      <c r="N18" s="6">
+        <v>63.35</v>
+      </c>
+      <c r="O18" s="6">
+        <v>14.92</v>
+      </c>
+      <c r="P18" s="6">
+        <v>13.08</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>52.23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="7">
+        <v>14056</v>
+      </c>
+      <c r="E19" s="7">
+        <v>19872354</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1413.8</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1395</v>
+      </c>
+      <c r="J19" s="6">
+        <v>1427</v>
+      </c>
+      <c r="K19" s="6">
+        <v>1455</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
+      <c r="M19" s="6">
+        <v>1428</v>
+      </c>
+      <c r="N19" s="6">
+        <v>51.51</v>
+      </c>
+      <c r="O19" s="6">
+        <v>10.86</v>
+      </c>
+      <c r="P19" s="6">
+        <v>12.23</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>53.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="7">
+        <v>93</v>
+      </c>
+      <c r="E20" s="7">
+        <v>134628</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1290</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1447.6</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1570</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1434</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1449</v>
+      </c>
+      <c r="K20" s="6">
+        <v>1468</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" s="6">
+        <v>1449</v>
+      </c>
+      <c r="N20" s="6">
+        <v>48.92</v>
+      </c>
+      <c r="O20" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="P20" s="6">
+        <v>11.98</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>54.87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="7">
+        <v>27739</v>
+      </c>
+      <c r="E21" s="7">
+        <v>39189098</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1412.8</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1600</v>
+      </c>
+      <c r="I21" s="6">
+        <v>1393</v>
+      </c>
+      <c r="J21" s="6">
+        <v>1420</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1445</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>1421</v>
+      </c>
+      <c r="N21" s="6">
+        <v>49.45</v>
+      </c>
+      <c r="O21" s="6">
+        <v>9.82</v>
+      </c>
+      <c r="P21" s="6">
+        <v>12.05</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>52.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5758</v>
+      </c>
+      <c r="E22" s="7">
+        <v>8173363</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1101</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1419.5</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1599</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1396</v>
+      </c>
+      <c r="J22" s="6">
+        <v>1425</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1451</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>1426</v>
+      </c>
+      <c r="N22" s="6">
+        <v>49.41</v>
+      </c>
+      <c r="O22" s="6">
+        <v>9.76</v>
+      </c>
+      <c r="P22" s="6">
+        <v>12.06</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>53.34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="6">
+        <f>AVERAGE(D2:D23)</f>
+        <v>17513</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" ref="E24:Q24" si="0">AVERAGE(E2:E23)</f>
+        <v>24797095.380952381</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>1124.4761904761904</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="0"/>
+        <v>1418.5142857142857</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>1591.7142857142858</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="0"/>
+        <v>1397.6666666666667</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="0"/>
+        <v>1425.9047619047619</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="0"/>
+        <v>1452.3095238095239</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="0"/>
+        <v>1427.0952380952381</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" si="0"/>
+        <v>51.401904761904767</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="0"/>
+        <v>10.743809523809521</v>
+      </c>
+      <c r="P24" s="6">
+        <f t="shared" si="0"/>
+        <v>12.220952380952383</v>
+      </c>
+      <c r="Q24" s="6">
+        <f t="shared" si="0"/>
+        <v>53.033333333333324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="6">
+        <f>SUM(D2:D22)</f>
+        <v>367773</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" ref="E25:Q25" si="1">SUM(E2:E22)</f>
+        <v>520739003</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>23614</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="1"/>
+        <v>29788.799999999999</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="1"/>
+        <v>33426</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>29351</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="1"/>
+        <v>29944</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="1"/>
+        <v>30498.5</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="1"/>
+        <v>29969</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="1"/>
+        <v>1079.44</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="1"/>
+        <v>225.61999999999992</v>
+      </c>
+      <c r="P25" s="6">
+        <f t="shared" si="1"/>
+        <v>256.64000000000004</v>
+      </c>
+      <c r="Q25" s="6">
+        <f t="shared" si="1"/>
+        <v>1113.6999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Cleaned documentation of classification workflow - Parsed NanoClass2 output
</commit_message>
<xml_diff>
--- a/results/data_summary.xlsx
+++ b/results/data_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/n_dombrowski_uva_nl/Documents/Teaching/2024/MicEco/data_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AFAA8DE-E3AE-4FC2-B638-C9FD3B05D3C4}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B569832-993B-4356-A5E4-DB4EE703DBFB}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="105" windowWidth="22650" windowHeight="15180" activeTab="1" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
+    <workbookView minimized="1" xWindow="2040" yWindow="210" windowWidth="22650" windowHeight="15180" activeTab="1" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="131">
   <si>
     <t>Barcode</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>not used for OUT table analysis</t>
   </si>
 </sst>
 </file>
@@ -837,7 +843,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A10" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1634,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C179779-2ECE-4B4E-99BE-E55FF918C4B5}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="A2" sqref="A2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1654,7 @@
     <col min="5" max="5" width="15.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>105</v>
       </c>
@@ -1664,30 +1670,33 @@
       <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -1699,12 +1708,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -1713,32 +1722,32 @@
         <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -1747,15 +1756,15 @@
         <v>13</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -1767,29 +1776,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1801,12 +1810,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1815,32 +1824,32 @@
         <v>11</v>
       </c>
       <c r="E10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
@@ -1852,12 +1861,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>3</v>
@@ -1866,15 +1875,15 @@
         <v>6</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
@@ -1886,29 +1895,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
@@ -1920,12 +1929,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
@@ -1937,29 +1946,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1971,12 +1980,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -1988,12 +1997,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
@@ -2005,27 +2014,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
+      <c r="F22" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
-    <sortCondition ref="C2:C22"/>
-    <sortCondition ref="D2:D22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
+    <sortCondition ref="C2:C21"/>
+    <sortCondition ref="D2:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,1309 +2045,1177 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760AAF3-A183-4133-AF68-A9D427019BD9}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="17" width="9" style="6"/>
+    <col min="2" max="2" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="6" t="s">
         <v>90</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="F1" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="B2" s="7">
         <v>60759</v>
       </c>
-      <c r="E2" s="5">
+      <c r="C2" s="7">
         <v>84356185</v>
       </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1388.4</v>
+      </c>
       <c r="F2" s="6">
-        <v>1</v>
+        <v>7133</v>
       </c>
       <c r="G2" s="6">
-        <v>1388.4</v>
+        <v>1409</v>
       </c>
       <c r="H2" s="6">
-        <v>7133</v>
+        <v>1432</v>
       </c>
       <c r="I2" s="6">
-        <v>1409</v>
+        <v>1456</v>
       </c>
       <c r="J2" s="6">
-        <v>1432</v>
+        <v>12.03</v>
       </c>
       <c r="K2" s="6">
-        <v>1456</v>
+        <v>52.74</v>
       </c>
       <c r="L2" s="6">
-        <v>0</v>
+        <v>49.43</v>
       </c>
       <c r="M2" s="6">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
         <v>1434</v>
       </c>
-      <c r="N2" s="6">
-        <v>49.43</v>
-      </c>
-      <c r="O2" s="6">
-        <v>9.8800000000000008</v>
-      </c>
-      <c r="P2" s="6">
-        <v>12.03</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>52.74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="7">
         <v>78436</v>
       </c>
-      <c r="E3" s="5">
+      <c r="C3" s="7">
         <v>106781562</v>
       </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1361.4</v>
+      </c>
       <c r="F3" s="6">
-        <v>3</v>
+        <v>3729</v>
       </c>
       <c r="G3" s="6">
-        <v>1361.4</v>
+        <v>1388</v>
       </c>
       <c r="H3" s="6">
-        <v>3729</v>
+        <v>1420</v>
       </c>
       <c r="I3" s="6">
-        <v>1388</v>
+        <v>1441</v>
       </c>
       <c r="J3" s="6">
-        <v>1420</v>
+        <v>12.06</v>
       </c>
       <c r="K3" s="6">
-        <v>1441</v>
+        <v>51.81</v>
       </c>
       <c r="L3" s="6">
-        <v>0</v>
+        <v>49.78</v>
       </c>
       <c r="M3" s="6">
+        <v>10.88</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
         <v>1423</v>
       </c>
-      <c r="N3" s="6">
-        <v>49.78</v>
-      </c>
-      <c r="O3" s="6">
-        <v>10.88</v>
-      </c>
-      <c r="P3" s="6">
-        <v>12.06</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>51.81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4" s="7">
         <v>28991</v>
       </c>
-      <c r="E4" s="5">
+      <c r="C4" s="7">
         <v>37302560</v>
       </c>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1286.7</v>
+      </c>
       <c r="F4" s="6">
-        <v>2</v>
+        <v>3497</v>
       </c>
       <c r="G4" s="6">
-        <v>1286.7</v>
+        <v>1282.5</v>
       </c>
       <c r="H4" s="6">
-        <v>3497</v>
+        <v>1427</v>
       </c>
       <c r="I4" s="6">
-        <v>1282.5</v>
+        <v>1457</v>
       </c>
       <c r="J4" s="6">
-        <v>1427</v>
+        <v>11.94</v>
       </c>
       <c r="K4" s="6">
-        <v>1457</v>
+        <v>53.06</v>
       </c>
       <c r="L4" s="6">
-        <v>0</v>
+        <v>48.4</v>
       </c>
       <c r="M4" s="6">
+        <v>9.34</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
         <v>1435</v>
       </c>
-      <c r="N4" s="6">
-        <v>48.4</v>
-      </c>
-      <c r="O4" s="6">
-        <v>9.34</v>
-      </c>
-      <c r="P4" s="6">
-        <v>11.94</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>53.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5" s="7">
         <v>4852</v>
       </c>
-      <c r="E5" s="5">
+      <c r="C5" s="7">
         <v>6716191</v>
       </c>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1384.2</v>
+      </c>
       <c r="F5" s="6">
-        <v>4</v>
+        <v>3120</v>
       </c>
       <c r="G5" s="6">
-        <v>1384.2</v>
+        <v>1391</v>
       </c>
       <c r="H5" s="6">
-        <v>3120</v>
+        <v>1427</v>
       </c>
       <c r="I5" s="6">
-        <v>1391</v>
+        <v>1457</v>
       </c>
       <c r="J5" s="6">
-        <v>1427</v>
+        <v>12.05</v>
       </c>
       <c r="K5" s="6">
-        <v>1457</v>
+        <v>52.56</v>
       </c>
       <c r="L5" s="6">
-        <v>0</v>
+        <v>49.61</v>
       </c>
       <c r="M5" s="6">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
         <v>1432</v>
       </c>
-      <c r="N5" s="6">
-        <v>49.61</v>
-      </c>
-      <c r="O5" s="6">
-        <v>10</v>
-      </c>
-      <c r="P5" s="6">
-        <v>12.05</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>52.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="7">
         <v>17883</v>
       </c>
-      <c r="E6" s="5">
+      <c r="C6" s="7">
         <v>24671910</v>
       </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1379.6</v>
+      </c>
       <c r="F6" s="6">
-        <v>2</v>
+        <v>3211</v>
       </c>
       <c r="G6" s="6">
-        <v>1379.6</v>
+        <v>1387</v>
       </c>
       <c r="H6" s="6">
-        <v>3211</v>
+        <v>1422</v>
       </c>
       <c r="I6" s="6">
-        <v>1387</v>
+        <v>1454</v>
       </c>
       <c r="J6" s="6">
-        <v>1422</v>
+        <v>12.06</v>
       </c>
       <c r="K6" s="6">
-        <v>1454</v>
+        <v>52.57</v>
       </c>
       <c r="L6" s="6">
-        <v>0</v>
+        <v>49.69</v>
       </c>
       <c r="M6" s="6">
+        <v>10.39</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6">
         <v>1427</v>
       </c>
-      <c r="N6" s="6">
-        <v>49.69</v>
-      </c>
-      <c r="O6" s="6">
-        <v>10.39</v>
-      </c>
-      <c r="P6" s="6">
-        <v>12.06</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>52.57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="B7" s="7">
         <v>18625</v>
       </c>
-      <c r="E7" s="5">
+      <c r="C7" s="7">
         <v>25580305</v>
       </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1373.4</v>
+      </c>
       <c r="F7" s="6">
-        <v>1</v>
+        <v>4541</v>
       </c>
       <c r="G7" s="6">
-        <v>1373.4</v>
+        <v>1384</v>
       </c>
       <c r="H7" s="6">
-        <v>4541</v>
+        <v>1411</v>
       </c>
       <c r="I7" s="6">
-        <v>1384</v>
+        <v>1448</v>
       </c>
       <c r="J7" s="6">
-        <v>1411</v>
+        <v>12.09</v>
       </c>
       <c r="K7" s="6">
-        <v>1448</v>
+        <v>52.39</v>
       </c>
       <c r="L7" s="6">
-        <v>0</v>
+        <v>49.98</v>
       </c>
       <c r="M7" s="6">
+        <v>10.48</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6">
         <v>1416</v>
       </c>
-      <c r="N7" s="6">
-        <v>49.98</v>
-      </c>
-      <c r="O7" s="6">
-        <v>10.48</v>
-      </c>
-      <c r="P7" s="6">
-        <v>12.09</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>52.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="B8" s="7">
         <v>12756</v>
       </c>
-      <c r="E8" s="5">
+      <c r="C8" s="7">
         <v>17124689</v>
       </c>
+      <c r="D8" s="6">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1342.5</v>
+      </c>
       <c r="F8" s="6">
-        <v>3</v>
+        <v>3522</v>
       </c>
       <c r="G8" s="6">
-        <v>1342.5</v>
+        <v>1376</v>
       </c>
       <c r="H8" s="6">
-        <v>3522</v>
+        <v>1407</v>
       </c>
       <c r="I8" s="6">
-        <v>1376</v>
+        <v>1435</v>
       </c>
       <c r="J8" s="6">
-        <v>1407</v>
+        <v>12.27</v>
       </c>
       <c r="K8" s="6">
-        <v>1435</v>
+        <v>53.33</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
+        <v>52.01</v>
       </c>
       <c r="M8" s="6">
+        <v>11.11</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6">
         <v>1411</v>
       </c>
-      <c r="N8" s="6">
-        <v>52.01</v>
-      </c>
-      <c r="O8" s="6">
-        <v>11.11</v>
-      </c>
-      <c r="P8" s="6">
-        <v>12.27</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>53.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
-      <c r="B9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="B9" s="7">
         <v>15666</v>
       </c>
-      <c r="E9" s="5">
+      <c r="C9" s="7">
         <v>21590962</v>
       </c>
+      <c r="D9" s="6">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1378.2</v>
+      </c>
       <c r="F9" s="6">
-        <v>4</v>
+        <v>4608</v>
       </c>
       <c r="G9" s="6">
-        <v>1378.2</v>
+        <v>1389</v>
       </c>
       <c r="H9" s="6">
-        <v>4608</v>
+        <v>1431</v>
       </c>
       <c r="I9" s="6">
-        <v>1389</v>
+        <v>1461</v>
       </c>
       <c r="J9" s="6">
-        <v>1431</v>
+        <v>12.25</v>
       </c>
       <c r="K9" s="6">
-        <v>1461</v>
+        <v>52.89</v>
       </c>
       <c r="L9" s="6">
-        <v>0</v>
+        <v>51.83</v>
       </c>
       <c r="M9" s="6">
+        <v>11.19</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
         <v>1436</v>
       </c>
-      <c r="N9" s="6">
-        <v>51.83</v>
-      </c>
-      <c r="O9" s="6">
-        <v>11.19</v>
-      </c>
-      <c r="P9" s="6">
-        <v>12.25</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>52.89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="B10" s="7">
         <v>15038</v>
       </c>
-      <c r="E10" s="5">
+      <c r="C10" s="7">
         <v>18630160</v>
       </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1238.9000000000001</v>
+      </c>
       <c r="F10" s="6">
-        <v>3</v>
+        <v>8085</v>
       </c>
       <c r="G10" s="6">
-        <v>1238.9000000000001</v>
+        <v>1130</v>
       </c>
       <c r="H10" s="6">
-        <v>8085</v>
+        <v>1389</v>
       </c>
       <c r="I10" s="6">
-        <v>1130</v>
+        <v>1422</v>
       </c>
       <c r="J10" s="6">
-        <v>1389</v>
+        <v>12.15</v>
       </c>
       <c r="K10" s="6">
-        <v>1422</v>
+        <v>53.4</v>
       </c>
       <c r="L10" s="6">
-        <v>0</v>
+        <v>50.94</v>
       </c>
       <c r="M10" s="6">
+        <v>10.57</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
         <v>1399</v>
       </c>
-      <c r="N10" s="6">
-        <v>50.94</v>
-      </c>
-      <c r="O10" s="6">
-        <v>10.57</v>
-      </c>
-      <c r="P10" s="6">
-        <v>12.15</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>53.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="B11" s="7">
         <v>7512</v>
       </c>
-      <c r="E11" s="5">
+      <c r="C11" s="7">
         <v>10025320</v>
       </c>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1334.6</v>
+      </c>
       <c r="F11" s="6">
-        <v>10</v>
+        <v>3657</v>
       </c>
       <c r="G11" s="6">
-        <v>1334.6</v>
+        <v>1367</v>
       </c>
       <c r="H11" s="6">
-        <v>3657</v>
+        <v>1404</v>
       </c>
       <c r="I11" s="6">
-        <v>1367</v>
+        <v>1442</v>
       </c>
       <c r="J11" s="6">
-        <v>1404</v>
+        <v>12.22</v>
       </c>
       <c r="K11" s="6">
-        <v>1442</v>
+        <v>52.34</v>
       </c>
       <c r="L11" s="6">
-        <v>0</v>
+        <v>51.73</v>
       </c>
       <c r="M11" s="6">
+        <v>11.09</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6">
         <v>1410</v>
       </c>
-      <c r="N11" s="6">
-        <v>51.73</v>
-      </c>
-      <c r="O11" s="6">
-        <v>11.09</v>
-      </c>
-      <c r="P11" s="6">
-        <v>12.22</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>52.34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="B12" s="7">
         <v>11099</v>
       </c>
-      <c r="E12" s="5">
+      <c r="C12" s="7">
         <v>15111939</v>
       </c>
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1361.6</v>
+      </c>
       <c r="F12" s="6">
-        <v>3</v>
+        <v>3140</v>
       </c>
       <c r="G12" s="6">
-        <v>1361.6</v>
+        <v>1384</v>
       </c>
       <c r="H12" s="6">
-        <v>3140</v>
+        <v>1429</v>
       </c>
       <c r="I12" s="6">
-        <v>1384</v>
+        <v>1457</v>
       </c>
       <c r="J12" s="6">
-        <v>1429</v>
+        <v>12.18</v>
       </c>
       <c r="K12" s="6">
-        <v>1457</v>
+        <v>54.52</v>
       </c>
       <c r="L12" s="6">
-        <v>0</v>
+        <v>51.08</v>
       </c>
       <c r="M12" s="6">
+        <v>10.6</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6">
         <v>1434</v>
       </c>
-      <c r="N12" s="6">
-        <v>51.08</v>
-      </c>
-      <c r="O12" s="6">
-        <v>10.6</v>
-      </c>
-      <c r="P12" s="6">
-        <v>12.18</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>54.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="B13" s="7">
         <v>6846</v>
       </c>
-      <c r="E13" s="5">
+      <c r="C13" s="7">
         <v>9383691</v>
       </c>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1370.7</v>
+      </c>
       <c r="F13" s="6">
-        <v>4</v>
+        <v>3144</v>
       </c>
       <c r="G13" s="6">
-        <v>1370.7</v>
+        <v>1384</v>
       </c>
       <c r="H13" s="6">
-        <v>3144</v>
+        <v>1420.5</v>
       </c>
       <c r="I13" s="6">
-        <v>1384</v>
+        <v>1455</v>
       </c>
       <c r="J13" s="6">
-        <v>1420.5</v>
+        <v>12.26</v>
       </c>
       <c r="K13" s="6">
-        <v>1455</v>
+        <v>52.58</v>
       </c>
       <c r="L13" s="6">
-        <v>0</v>
+        <v>51.87</v>
       </c>
       <c r="M13" s="6">
+        <v>11.37</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
         <v>1427</v>
       </c>
-      <c r="N13" s="6">
-        <v>51.87</v>
-      </c>
-      <c r="O13" s="6">
-        <v>11.37</v>
-      </c>
-      <c r="P13" s="6">
-        <v>12.26</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>52.58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
-      <c r="B14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="B14" s="7">
         <v>14785</v>
       </c>
-      <c r="E14" s="5">
+      <c r="C14" s="7">
         <v>20509267</v>
       </c>
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1387.2</v>
+      </c>
       <c r="F14" s="6">
-        <v>2</v>
+        <v>3254</v>
       </c>
       <c r="G14" s="6">
-        <v>1387.2</v>
+        <v>1404</v>
       </c>
       <c r="H14" s="6">
-        <v>3254</v>
+        <v>1435</v>
       </c>
       <c r="I14" s="6">
-        <v>1404</v>
+        <v>1463</v>
       </c>
       <c r="J14" s="6">
-        <v>1435</v>
+        <v>12.23</v>
       </c>
       <c r="K14" s="6">
-        <v>1463</v>
+        <v>53.19</v>
       </c>
       <c r="L14" s="6">
-        <v>0</v>
+        <v>51.61</v>
       </c>
       <c r="M14" s="6">
+        <v>10.59</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
         <v>1439</v>
       </c>
-      <c r="N14" s="6">
-        <v>51.61</v>
-      </c>
-      <c r="O14" s="6">
-        <v>10.59</v>
-      </c>
-      <c r="P14" s="6">
-        <v>12.23</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>53.19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
-      <c r="B15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="B15" s="7">
         <v>18654</v>
       </c>
-      <c r="E15" s="5">
+      <c r="C15" s="7">
         <v>25863501</v>
       </c>
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1386.5</v>
+      </c>
       <c r="F15" s="6">
-        <v>3</v>
+        <v>4420</v>
       </c>
       <c r="G15" s="6">
-        <v>1386.5</v>
+        <v>1405</v>
       </c>
       <c r="H15" s="6">
-        <v>4420</v>
+        <v>1435</v>
       </c>
       <c r="I15" s="6">
-        <v>1405</v>
+        <v>1457</v>
       </c>
       <c r="J15" s="6">
-        <v>1435</v>
+        <v>12.22</v>
       </c>
       <c r="K15" s="6">
-        <v>1457</v>
+        <v>53.5</v>
       </c>
       <c r="L15" s="6">
-        <v>0</v>
+        <v>51.58</v>
       </c>
       <c r="M15" s="6">
+        <v>10.85</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
         <v>1438</v>
       </c>
-      <c r="N15" s="6">
-        <v>51.58</v>
-      </c>
-      <c r="O15" s="6">
-        <v>10.85</v>
-      </c>
-      <c r="P15" s="6">
-        <v>12.22</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>53.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
-      <c r="B16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="B16" s="7">
         <v>16957</v>
       </c>
-      <c r="E16" s="5">
+      <c r="C16" s="7">
         <v>23494889</v>
       </c>
+      <c r="D16" s="6">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1385.6</v>
+      </c>
       <c r="F16" s="6">
-        <v>3</v>
+        <v>3576</v>
       </c>
       <c r="G16" s="6">
-        <v>1385.6</v>
+        <v>1397</v>
       </c>
       <c r="H16" s="6">
-        <v>3576</v>
+        <v>1439</v>
       </c>
       <c r="I16" s="6">
-        <v>1397</v>
+        <v>1467</v>
       </c>
       <c r="J16" s="6">
-        <v>1439</v>
+        <v>12.23</v>
       </c>
       <c r="K16" s="6">
-        <v>1467</v>
+        <v>53.14</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>51.6</v>
       </c>
       <c r="M16" s="6">
+        <v>10.55</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
         <v>1443</v>
       </c>
-      <c r="N16" s="6">
-        <v>51.6</v>
-      </c>
-      <c r="O16" s="6">
-        <v>10.55</v>
-      </c>
-      <c r="P16" s="6">
-        <v>12.23</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>53.14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="B17" s="7">
         <v>30101</v>
       </c>
-      <c r="E17" s="5">
+      <c r="C17" s="7">
         <v>40492140</v>
       </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1345.2</v>
+      </c>
       <c r="F17" s="6">
-        <v>1</v>
+        <v>4706</v>
       </c>
       <c r="G17" s="6">
-        <v>1345.2</v>
+        <v>1383</v>
       </c>
       <c r="H17" s="6">
-        <v>4706</v>
+        <v>1424</v>
       </c>
       <c r="I17" s="6">
-        <v>1383</v>
+        <v>1452</v>
       </c>
       <c r="J17" s="6">
-        <v>1424</v>
+        <v>12.2</v>
       </c>
       <c r="K17" s="6">
-        <v>1452</v>
+        <v>52.96</v>
       </c>
       <c r="L17" s="6">
-        <v>0</v>
+        <v>51.29</v>
       </c>
       <c r="M17" s="6">
+        <v>10.98</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6">
         <v>1429</v>
       </c>
-      <c r="N17" s="6">
-        <v>51.29</v>
-      </c>
-      <c r="O17" s="6">
-        <v>10.98</v>
-      </c>
-      <c r="P17" s="6">
-        <v>12.2</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>52.96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="B18" s="7">
         <v>3</v>
       </c>
-      <c r="E18" s="5">
+      <c r="C18" s="7">
         <v>4404</v>
       </c>
+      <c r="D18" s="6">
+        <v>1421</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1468</v>
+      </c>
       <c r="F18" s="6">
-        <v>1421</v>
+        <v>1518</v>
       </c>
       <c r="G18" s="6">
-        <v>1468</v>
+        <v>1443</v>
       </c>
       <c r="H18" s="6">
-        <v>1518</v>
+        <v>1465</v>
       </c>
       <c r="I18" s="6">
-        <v>1443</v>
+        <v>1491.5</v>
       </c>
       <c r="J18" s="6">
+        <v>13.08</v>
+      </c>
+      <c r="K18" s="6">
+        <v>52.23</v>
+      </c>
+      <c r="L18" s="6">
+        <v>63.35</v>
+      </c>
+      <c r="M18" s="6">
+        <v>14.92</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0</v>
+      </c>
+      <c r="O18" s="6">
         <v>1465</v>
       </c>
-      <c r="K18" s="6">
-        <v>1491.5</v>
-      </c>
-      <c r="L18" s="6">
-        <v>0</v>
-      </c>
-      <c r="M18" s="6">
-        <v>1465</v>
-      </c>
-      <c r="N18" s="6">
-        <v>63.35</v>
-      </c>
-      <c r="O18" s="6">
-        <v>14.92</v>
-      </c>
-      <c r="P18" s="6">
-        <v>13.08</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>52.23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="B19" s="7">
         <v>16945</v>
       </c>
-      <c r="E19" s="5">
+      <c r="C19" s="7">
         <v>22338534</v>
       </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1318.3</v>
+      </c>
       <c r="F19" s="6">
-        <v>3</v>
+        <v>4814</v>
       </c>
       <c r="G19" s="6">
-        <v>1318.3</v>
+        <v>1348</v>
       </c>
       <c r="H19" s="6">
-        <v>4814</v>
+        <v>1422</v>
       </c>
       <c r="I19" s="6">
-        <v>1348</v>
+        <v>1453</v>
       </c>
       <c r="J19" s="6">
-        <v>1422</v>
+        <v>12.18</v>
       </c>
       <c r="K19" s="6">
-        <v>1453</v>
+        <v>53.01</v>
       </c>
       <c r="L19" s="6">
-        <v>0</v>
+        <v>51.17</v>
       </c>
       <c r="M19" s="6">
+        <v>10.79</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0</v>
+      </c>
+      <c r="O19" s="6">
         <v>1429</v>
       </c>
-      <c r="N19" s="6">
-        <v>51.17</v>
-      </c>
-      <c r="O19" s="6">
-        <v>10.79</v>
-      </c>
-      <c r="P19" s="6">
-        <v>12.18</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>53.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="B20" s="7">
         <v>109</v>
       </c>
-      <c r="E20" s="5">
+      <c r="C20" s="7">
         <v>142007</v>
       </c>
+      <c r="D20" s="6">
+        <v>41</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1302.8</v>
+      </c>
       <c r="F20" s="6">
-        <v>41</v>
+        <v>1595</v>
       </c>
       <c r="G20" s="6">
-        <v>1302.8</v>
+        <v>1430</v>
       </c>
       <c r="H20" s="6">
-        <v>1595</v>
+        <v>1449</v>
       </c>
       <c r="I20" s="6">
-        <v>1430</v>
+        <v>1470</v>
       </c>
       <c r="J20" s="6">
-        <v>1449</v>
+        <v>11.89</v>
       </c>
       <c r="K20" s="6">
-        <v>1470</v>
+        <v>54.7</v>
       </c>
       <c r="L20" s="6">
-        <v>0</v>
+        <v>48.55</v>
       </c>
       <c r="M20" s="6">
+        <v>9.59</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0</v>
+      </c>
+      <c r="O20" s="6">
         <v>1455</v>
       </c>
-      <c r="N20" s="6">
-        <v>48.55</v>
-      </c>
-      <c r="O20" s="6">
-        <v>9.59</v>
-      </c>
-      <c r="P20" s="6">
-        <v>11.89</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>54.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>82</v>
       </c>
-      <c r="B21" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="B21" s="7">
         <v>31428</v>
       </c>
-      <c r="E21" s="5">
+      <c r="C21" s="7">
         <v>42360283</v>
       </c>
+      <c r="D21" s="6">
+        <v>3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1347.9</v>
+      </c>
       <c r="F21" s="6">
-        <v>3</v>
+        <v>4211</v>
       </c>
       <c r="G21" s="6">
-        <v>1347.9</v>
+        <v>1388</v>
       </c>
       <c r="H21" s="6">
-        <v>4211</v>
+        <v>1422</v>
       </c>
       <c r="I21" s="6">
-        <v>1388</v>
+        <v>1449</v>
       </c>
       <c r="J21" s="6">
-        <v>1422</v>
+        <v>12.02</v>
       </c>
       <c r="K21" s="6">
-        <v>1449</v>
+        <v>52.9</v>
       </c>
       <c r="L21" s="6">
-        <v>0</v>
+        <v>49.25</v>
       </c>
       <c r="M21" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
         <v>1426</v>
       </c>
-      <c r="N21" s="6">
-        <v>49.25</v>
-      </c>
-      <c r="O21" s="6">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P21" s="6">
-        <v>12.02</v>
-      </c>
-      <c r="Q21" s="6">
-        <v>52.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="B22" s="7">
         <v>6169</v>
       </c>
-      <c r="E22" s="5">
+      <c r="C22" s="7">
         <v>8551391</v>
       </c>
+      <c r="D22" s="6">
+        <v>4</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1386.2</v>
+      </c>
       <c r="F22" s="6">
-        <v>4</v>
+        <v>3117</v>
       </c>
       <c r="G22" s="6">
-        <v>1386.2</v>
+        <v>1398</v>
       </c>
       <c r="H22" s="6">
-        <v>3117</v>
+        <v>1426</v>
       </c>
       <c r="I22" s="6">
-        <v>1398</v>
+        <v>1454</v>
       </c>
       <c r="J22" s="6">
-        <v>1426</v>
+        <v>12.01</v>
       </c>
       <c r="K22" s="6">
-        <v>1454</v>
+        <v>53.32</v>
       </c>
       <c r="L22" s="6">
-        <v>0</v>
+        <v>49.18</v>
       </c>
       <c r="M22" s="6">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
         <v>1429</v>
       </c>
-      <c r="N22" s="6">
-        <v>49.18</v>
-      </c>
-      <c r="O22" s="6">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="P22" s="6">
-        <v>12.01</v>
-      </c>
-      <c r="Q22" s="6">
-        <v>53.32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
+      <c r="B24" s="6">
+        <f>AVERAGE(B2:B23)</f>
+        <v>19695.904761904763</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" ref="C24:K24" si="0">AVERAGE(C2:C23)</f>
+        <v>26715804.285714287</v>
+      </c>
       <c r="D24" s="6">
-        <f>AVERAGE(D2:D23)</f>
-        <v>19695.904761904763</v>
+        <f t="shared" si="0"/>
+        <v>72.428571428571431</v>
       </c>
       <c r="E24" s="6">
-        <f t="shared" ref="E24:Q24" si="0">AVERAGE(E2:E23)</f>
-        <v>26715804.285714287</v>
+        <f t="shared" si="0"/>
+        <v>1358.4714285714285</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
-        <v>72.428571428571431</v>
+        <v>3933.2380952380954</v>
       </c>
       <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>1358.4714285714285</v>
+        <v>1374.6428571428571</v>
       </c>
       <c r="H24" s="6">
         <f t="shared" si="0"/>
-        <v>3933.2380952380954</v>
+        <v>1425.547619047619</v>
       </c>
       <c r="I24" s="6">
         <f t="shared" si="0"/>
-        <v>1374.6428571428571</v>
+        <v>1454.3571428571429</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" si="0"/>
-        <v>1425.547619047619</v>
+        <v>12.172380952380951</v>
       </c>
       <c r="K24" s="6">
         <f t="shared" si="0"/>
-        <v>1454.3571428571429</v>
+        <v>53.006666666666661</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>AVERAGE(L2:L23)</f>
+        <v>51.139523809523816</v>
       </c>
       <c r="M24" s="6">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(M2:M23)</f>
+        <v>10.698571428571428</v>
+      </c>
+      <c r="N24" s="6">
+        <f>AVERAGE(N2:N23)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <f>AVERAGE(O2:O23)</f>
         <v>1430.3333333333333</v>
       </c>
-      <c r="N24" s="6">
-        <f t="shared" si="0"/>
-        <v>51.139523809523816</v>
-      </c>
-      <c r="O24" s="6">
-        <f t="shared" si="0"/>
-        <v>10.698571428571428</v>
-      </c>
-      <c r="P24" s="6">
-        <f t="shared" si="0"/>
-        <v>12.172380952380951</v>
-      </c>
-      <c r="Q24" s="6">
-        <f t="shared" si="0"/>
-        <v>53.006666666666661</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>128</v>
       </c>
+      <c r="B25" s="7">
+        <f>SUM(B2:B22)</f>
+        <v>413614</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" ref="C25:K25" si="1">SUM(C2:C22)</f>
+        <v>561031890</v>
+      </c>
       <c r="D25" s="5">
-        <f>SUM(D2:D22)</f>
-        <v>413614</v>
+        <f t="shared" si="1"/>
+        <v>1521</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" ref="E25:Q25" si="1">SUM(E2:E22)</f>
-        <v>561031890</v>
+        <f t="shared" si="1"/>
+        <v>28527.9</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="1"/>
-        <v>1521</v>
+        <v>82598</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="1"/>
-        <v>28527.9</v>
+        <v>28867.5</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="1"/>
-        <v>82598</v>
+        <v>29936.5</v>
       </c>
       <c r="I25" s="5">
         <f t="shared" si="1"/>
-        <v>28867.5</v>
+        <v>30541.5</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="1"/>
-        <v>29936.5</v>
+        <v>255.61999999999998</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>30541.5</v>
+        <v>1113.1399999999999</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(L2:L22)</f>
+        <v>1073.93</v>
       </c>
       <c r="M25" s="5">
-        <f t="shared" si="1"/>
+        <f>SUM(M2:M22)</f>
+        <v>224.67</v>
+      </c>
+      <c r="N25" s="5">
+        <f>SUM(N2:N22)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <f>SUM(O2:O22)</f>
         <v>30037</v>
-      </c>
-      <c r="N25" s="5">
-        <f t="shared" si="1"/>
-        <v>1073.93</v>
-      </c>
-      <c r="O25" s="5">
-        <f t="shared" si="1"/>
-        <v>224.67</v>
-      </c>
-      <c r="P25" s="5">
-        <f t="shared" si="1"/>
-        <v>255.61999999999998</v>
-      </c>
-      <c r="Q25" s="5">
-        <f t="shared" si="1"/>
-        <v>1113.1399999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3349,7 +3229,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Wrote code to analyse OTU table - Prettified website layout
</commit_message>
<xml_diff>
--- a/results/data_summary.xlsx
+++ b/results/data_summary.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/n_dombrowski_uva_nl/Documents/Teaching/2024/MicEco/data_analysis/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B569832-993B-4356-A5E4-DB4EE703DBFB}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{C53CF6CE-474C-B14A-876A-FC82B9703F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD6445F-14CD-4E24-A7F0-E412F1A793BE}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2040" yWindow="210" windowWidth="22650" windowHeight="15180" activeTab="1" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
+    <workbookView xWindow="1020" yWindow="240" windowWidth="17775" windowHeight="13335" activeTab="2" xr2:uid="{FF4F9962-2689-834F-82B6-CE6F3C06F42E}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="mapping_file" sheetId="3" r:id="rId2"/>
-    <sheet name="seqkit_raw" sheetId="2" r:id="rId3"/>
-    <sheet name="seqkit_filtered" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="seqkit_raw" sheetId="2" r:id="rId4"/>
+    <sheet name="seqkit_filtered" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="153">
   <si>
     <t>Barcode</t>
   </si>
@@ -432,6 +433,72 @@
   </si>
   <si>
     <t>not used for OUT table analysis</t>
+  </si>
+  <si>
+    <t>Acetivibrio</t>
+  </si>
+  <si>
+    <t>Ruminiclostridium</t>
+  </si>
+  <si>
+    <t>Ruminococcus</t>
+  </si>
+  <si>
+    <t>Cellulosilyticum</t>
+  </si>
+  <si>
+    <t>Sulfurimonas</t>
+  </si>
+  <si>
+    <t>Candidatus_Competibacter</t>
+  </si>
+  <si>
+    <t>Cohaesibacter</t>
+  </si>
+  <si>
+    <t>Defluviicoccus</t>
+  </si>
+  <si>
+    <t>Spirochaeta_2</t>
+  </si>
+  <si>
+    <t>JTB215</t>
+  </si>
+  <si>
+    <t>Marinifilum</t>
+  </si>
+  <si>
+    <t>Nitrospina</t>
+  </si>
+  <si>
+    <t>Candidatus_Nitrotoga</t>
+  </si>
+  <si>
+    <t>Thioalkalispira_Sulfurivermis</t>
+  </si>
+  <si>
+    <t>Endomicrobium</t>
+  </si>
+  <si>
+    <t>Stappia</t>
+  </si>
+  <si>
+    <t>SEEP_SRB1</t>
+  </si>
+  <si>
+    <t>SM23_31</t>
+  </si>
+  <si>
+    <t>Demequina</t>
+  </si>
+  <si>
+    <t>Thiohalocapsa</t>
+  </si>
+  <si>
+    <t>Pelagibius</t>
+  </si>
+  <si>
+    <t>Anaerophaga</t>
   </si>
 </sst>
 </file>
@@ -485,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -505,6 +572,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1642,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C179779-2ECE-4B4E-99BE-E55FF918C4B5}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2044,6 +2117,422 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4CD416-170B-4599-BEBA-6C0DC9F9338A}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="8">
+        <v>-6.0595999999999997</v>
+      </c>
+      <c r="C1" s="8">
+        <v>1.5066999999999999</v>
+      </c>
+      <c r="D1" s="9">
+        <v>5.7741999999999997E-5</v>
+      </c>
+      <c r="E1" s="8">
+        <v>2.5872E-3</v>
+      </c>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="8">
+        <v>-4.6566000000000001</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2.9236000000000003E-4</v>
+      </c>
+      <c r="E2" s="8">
+        <v>6.117E-3</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="8">
+        <v>-4.1595000000000004</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>6.6582999999999996E-5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2.5872E-3</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="8">
+        <v>-4.1102999999999996</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1.0665</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1.1616999999999999E-4</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3.6105999999999998E-3</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="8">
+        <v>-3.9967999999999999</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.1024</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.8826999999999998E-4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6.117E-3</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="8">
+        <v>-3.7059000000000002</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.0341</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3.3870999999999999E-4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>6.5807000000000001E-3</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="8">
+        <v>-3.5270000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.159</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2.3421000000000002E-3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3.3529000000000003E-2</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-3.0333000000000001</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.0239</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3.0504E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.9510999999999998E-2</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="8">
+        <v>-2.4834999999999998</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.64554</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1.1947000000000001E-4</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3.6105999999999998E-3</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="8">
+        <v>-2.1795</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.73275000000000001</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2.9350999999999999E-3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>3.9510999999999998E-2</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="8">
+        <v>-2.1271</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.62905999999999995</v>
+      </c>
+      <c r="D11" s="9">
+        <v>7.2128000000000003E-4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1.2262E-2</v>
+      </c>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="8">
+        <v>-1.7645999999999999</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.43389</v>
+      </c>
+      <c r="D12" s="9">
+        <v>4.7605000000000002E-5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2.5872E-3</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1.1762999999999999</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.37728</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.8213000000000001E-3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2.9139999999999999E-2</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1.4477</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.47144000000000003</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2.1351E-3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3.2264000000000001E-2</v>
+      </c>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1.4937</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.39095000000000002</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1.3312999999999999E-4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3.6210999999999999E-3</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.9475</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.52270000000000005</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1.9464999999999999E-4</v>
+      </c>
+      <c r="E16" s="8">
+        <v>4.8130999999999998E-3</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3.2797000000000001</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.1296999999999999</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3.6946000000000001E-3</v>
+      </c>
+      <c r="E17" s="8">
+        <v>4.5678000000000003E-2</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3.7709999999999999</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1.0652999999999999</v>
+      </c>
+      <c r="D18" s="9">
+        <v>4.0055000000000001E-4</v>
+      </c>
+      <c r="E18" s="8">
+        <v>7.2633999999999997E-3</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="8">
+        <v>6.8353999999999999</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.81381000000000003</v>
+      </c>
+      <c r="D19" s="9">
+        <v>4.4931000000000002E-17</v>
+      </c>
+      <c r="E19" s="9">
+        <v>6.1106999999999997E-15</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="8">
+        <v>9.1599000000000004</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1.5124</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1.3922E-9</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1.2623000000000001E-7</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.99899000000000004</v>
+      </c>
+      <c r="D21" s="9">
+        <v>3.2827999999999998E-20</v>
+      </c>
+      <c r="E21" s="9">
+        <v>8.9293000000000007E-18</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="8">
+        <v>9.4512999999999998</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1.5757000000000001</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1.9946000000000001E-9</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1.3563E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E22">
+    <sortCondition ref="B1:B22"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760AAF3-A183-4133-AF68-A9D427019BD9}">
   <dimension ref="A1:O25"/>
   <sheetViews>
@@ -2051,7 +2540,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3224,12 +3713,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64606F4B-74B8-49A9-B4AF-97DC0E2C0EB5}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>